<commit_message>
adding updated file in develop branch
</commit_message>
<xml_diff>
--- a/INDIA-WeatherMapping.xlsx
+++ b/INDIA-WeatherMapping.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EDS_Projects\S2502 Citi\Git\ClimateZoneFinder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EDS_Projects\S25129_Climate Zone Finder\git\ClimateZoneFinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1059A03D-4D5E-4691-93D8-99F8988ECF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B88412-8F72-4AA5-B863-B8137AD7BA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF33B568-C928-4D88-B064-E16121AC4B71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$1:$L$730</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5633" uniqueCount="1240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5729" uniqueCount="1252">
   <si>
     <t>Country</t>
   </si>
@@ -3759,6 +3760,42 @@
   </si>
   <si>
     <t>https://climate.onebuilding.org/WMO_Region_2_Asia/IND_India/DL_Delhi/IND_DL_New.Delhi-Safdarjung.AP.421820_TMYx.zip</t>
+  </si>
+  <si>
+    <t>Sub-tropic</t>
+  </si>
+  <si>
+    <t>25°C</t>
+  </si>
+  <si>
+    <t>Jaiselmer</t>
+  </si>
+  <si>
+    <t>Sub tropic</t>
+  </si>
+  <si>
+    <t>Warm &amp; Humid</t>
+  </si>
+  <si>
+    <t>Tropic</t>
+  </si>
+  <si>
+    <t>27°C</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Shillong</t>
+  </si>
+  <si>
+    <t>23°C</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>Sub -Tropic</t>
   </si>
 </sst>
 </file>
@@ -4204,8 +4241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C3B464-FF04-4353-A8AE-0A433A2C5F28}">
   <dimension ref="A1:O730"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="94" workbookViewId="0">
+      <selection activeCell="F158" sqref="F158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30360,4 +30397,403 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFB59CD-D0BE-4D5D-92F1-FE0536BDAE88}">
+  <dimension ref="A1:E48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" t="s">
+        <v>769</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>769</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C2" t="s">
+        <v>769</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B3" t="s">
+        <v>582</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B5" t="s">
+        <v>752</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>769</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D6" t="s">
+        <v>772</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C7" t="s">
+        <v>772</v>
+      </c>
+      <c r="D7" t="s">
+        <v>772</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B8" t="s">
+        <v>617</v>
+      </c>
+      <c r="C8" t="s">
+        <v>767</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>582</v>
+      </c>
+      <c r="B9" t="s">
+        <v>423</v>
+      </c>
+      <c r="C9" t="s">
+        <v>767</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B10" t="s">
+        <v>362</v>
+      </c>
+      <c r="C10" t="s">
+        <v>767</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>767</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" t="s">
+        <v>767</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1251</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>